<commit_message>
updated taskallocation chart and mysqlexport file
</commit_message>
<xml_diff>
--- a/com.blackout.solarpanelcalculator/docs/Task Allocation Chart.xlsx
+++ b/com.blackout.solarpanelcalculator/docs/Task Allocation Chart.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="93">
   <si>
     <t>Aaron</t>
   </si>
@@ -262,12 +262,6 @@
     <t>improve UI layout</t>
   </si>
   <si>
-    <t>similar system generation</t>
-  </si>
-  <si>
-    <t>More junit tests (e.g.for payback year)</t>
-  </si>
-  <si>
     <t>more code refactoring</t>
   </si>
   <si>
@@ -314,6 +308,21 @@
   </si>
   <si>
     <t>More junit tests ( for CityDAO class, CalculationFormulas class)</t>
+  </si>
+  <si>
+    <t>More junit tests (for CityDAO class, CalculationFormulas class)</t>
+  </si>
+  <si>
+    <t>implement validate user input function</t>
+  </si>
+  <si>
+    <t>code refactoring</t>
+  </si>
+  <si>
+    <t>similar system generation in web app (optional)</t>
+  </si>
+  <si>
+    <t>similar system generation in desktop app (optional)</t>
   </si>
 </sst>
 </file>
@@ -326,7 +335,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -340,11 +349,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -377,7 +381,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -399,6 +403,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -452,7 +462,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -462,16 +472,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -495,22 +502,22 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -522,17 +529,17 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -905,67 +912,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T70"/>
+  <dimension ref="A1:T71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" style="22" customWidth="1"/>
-    <col min="3" max="3" width="82.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="4" customWidth="1"/>
-    <col min="7" max="20" width="17.109375" style="4" customWidth="1"/>
-    <col min="21" max="16384" width="17.109375" style="4"/>
+    <col min="1" max="1" width="17.44140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" style="21" customWidth="1"/>
+    <col min="3" max="3" width="82.21875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="3" customWidth="1"/>
+    <col min="7" max="20" width="17.109375" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="17.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>41163</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -974,7 +983,7 @@
       <c r="D2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -998,10 +1007,10 @@
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>41163</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1010,32 +1019,32 @@
       <c r="D3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
     </row>
     <row r="4" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>41163</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1044,32 +1053,32 @@
       <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>41163</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1078,32 +1087,32 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
     </row>
     <row r="6" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <v>41163</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1112,213 +1121,213 @@
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
     </row>
     <row r="7" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>41163</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="7" t="s">
         <v>33</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="5"/>
-      <c r="R7" s="5"/>
-      <c r="S7" s="5"/>
-      <c r="T7" s="5"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
     </row>
     <row r="8" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="19">
         <v>41163</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
     </row>
     <row r="9" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="19">
         <v>41163</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
     </row>
     <row r="10" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="19">
         <v>41163</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
     </row>
     <row r="11" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <v>41163</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5"/>
-      <c r="R11" s="5"/>
-      <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
     </row>
     <row r="12" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <v>41163</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1334,25 +1343,25 @@
       <c r="T12" s="2"/>
     </row>
     <row r="13" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="19">
         <v>41163</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="4"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1368,23 +1377,23 @@
       <c r="T13" s="2"/>
     </row>
     <row r="14" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="20">
+      <c r="B14" s="19">
         <v>41163</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E14" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="5"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1400,23 +1409,23 @@
       <c r="T14" s="2"/>
     </row>
     <row r="15" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="20">
+      <c r="B15" s="19">
         <v>41163</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="8" t="s">
         <v>33</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="5"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1432,25 +1441,25 @@
       <c r="T15" s="2"/>
     </row>
     <row r="16" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="21">
+      <c r="B16" s="20">
         <v>41163</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1466,25 +1475,25 @@
       <c r="T16" s="2"/>
     </row>
     <row r="17" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="21">
+      <c r="B17" s="20">
         <v>41163</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1500,23 +1509,23 @@
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="20">
         <v>41170</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1532,25 +1541,25 @@
       <c r="T18" s="2"/>
     </row>
     <row r="19" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="19">
         <v>41170</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="4"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1566,607 +1575,647 @@
       <c r="T19" s="2"/>
     </row>
     <row r="20" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="20">
+      <c r="B20" s="19">
         <v>41170</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="20">
+      <c r="B21" s="19">
         <v>41170</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="20">
+      <c r="B22" s="19">
         <v>41170</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="5"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="20">
+      <c r="B23" s="19">
         <v>41170</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="7" t="s">
+      <c r="D23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="20">
+      <c r="B24" s="19">
         <v>41170</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="5"/>
+      <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="20">
+      <c r="B25" s="19">
         <v>41170</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="7" t="s">
+      <c r="D25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="6" t="s">
         <v>24</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="5"/>
+      <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="20">
+      <c r="B26" s="19">
         <v>41170</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="9" t="s">
+      <c r="D26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="20">
+      <c r="B27" s="19">
         <v>41170</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="5" t="s">
+      <c r="E27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="5" t="s">
+      <c r="G27" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H27" s="4" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="20">
+      <c r="B28" s="19">
         <v>41170</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" s="5" t="s">
+      <c r="E28" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="5" t="s">
+      <c r="H28" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="19">
+        <v>41170</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="19"/>
+      <c r="C31" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="15"/>
+      <c r="E31" s="25"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E38" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="12"/>
+      <c r="B39" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="12"/>
+      <c r="B43" s="19">
+        <v>41184</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="12"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="12"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="12"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E47" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="12"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="22" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="B29" s="20">
-        <v>41170</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="20"/>
-      <c r="C31" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="16"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C32" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="26" t="s">
+      <c r="E49" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="13"/>
-      <c r="B37" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C37" s="5" t="s">
+    </row>
+    <row r="50" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E50" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="12"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13"/>
-      <c r="B38" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" s="26" t="s">
+      <c r="E53" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13"/>
-      <c r="B39" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="26" t="s">
+    <row r="54" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E54" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E40" s="26" t="s">
+    <row r="55" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="C55" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E55" s="24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13"/>
-      <c r="B41" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="20">
-        <v>41184</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="13"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="13"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="E45" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E46" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E48" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="E50" s="26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="20"/>
-    </row>
-    <row r="52" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="20"/>
-    </row>
-    <row r="53" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="20"/>
-    </row>
-    <row r="54" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-    </row>
-    <row r="55" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-    </row>
     <row r="56" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+      <c r="A56" s="12"/>
     </row>
     <row r="57" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+      <c r="A57" s="12"/>
     </row>
     <row r="58" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
+      <c r="A58" s="12"/>
     </row>
     <row r="59" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
+      <c r="A59" s="12"/>
     </row>
     <row r="60" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+      <c r="A60" s="12"/>
     </row>
     <row r="61" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
+      <c r="A61" s="12"/>
     </row>
     <row r="62" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
+      <c r="A62" s="12"/>
     </row>
     <row r="63" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="13"/>
+      <c r="A63" s="12"/>
     </row>
     <row r="64" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
+      <c r="A64" s="12"/>
     </row>
     <row r="65" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+      <c r="A65" s="12"/>
     </row>
     <row r="66" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+      <c r="A66" s="12"/>
     </row>
     <row r="67" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+      <c r="A67" s="12"/>
     </row>
     <row r="68" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+      <c r="A68" s="12"/>
     </row>
     <row r="69" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+      <c r="A69" s="12"/>
     </row>
     <row r="70" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+      <c r="A70" s="12"/>
+    </row>
+    <row r="71" spans="1:1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Re-added Felix's Datatables and minor documentation
I don't know how they disappeared but here they are again.
</commit_message>
<xml_diff>
--- a/com.blackout.solarpanelcalculator/docs/Task Allocation Chart.xlsx
+++ b/com.blackout.solarpanelcalculator/docs/Task Allocation Chart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="123820"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2880" windowWidth="21960" windowHeight="8952"/>
+    <workbookView xWindow="0" yWindow="2880" windowWidth="20730" windowHeight="8955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,7 @@
     <definedName name="guhiz91c7yia">Sheet1!$C$1</definedName>
     <definedName name="nyddfya4pgcl">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="103">
   <si>
     <t>Aaron</t>
   </si>
@@ -344,9 +343,6 @@
     <t>implement optimal degrees based on user location</t>
   </si>
   <si>
-    <t>junit tests</t>
-  </si>
-  <si>
     <t>selenium tests</t>
   </si>
   <si>
@@ -354,19 +350,22 @@
   </si>
   <si>
     <t>polish montly generation chart and payback time line chart (optional)</t>
+  </si>
+  <si>
+    <t>refine junit tests</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -747,7 +746,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -782,7 +780,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -955,28 +952,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T80"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" style="20" customWidth="1"/>
-    <col min="3" max="3" width="82.33203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.109375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="3" customWidth="1"/>
-    <col min="7" max="20" width="17.109375" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="17.109375" style="3"/>
+    <col min="1" max="1" width="17.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="20" customWidth="1"/>
+    <col min="3" max="3" width="82.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="3" customWidth="1"/>
+    <col min="7" max="20" width="17.140625" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="17.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="15">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1014,7 +1011,7 @@
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
     </row>
-    <row r="2" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="14.25">
       <c r="A2" s="9" t="s">
         <v>43</v>
       </c>
@@ -1050,7 +1047,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="12.75" customHeight="1">
       <c r="A3" s="10" t="s">
         <v>43</v>
       </c>
@@ -1084,7 +1081,7 @@
       <c r="S3" s="4"/>
       <c r="T3" s="4"/>
     </row>
-    <row r="4" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="12.75" customHeight="1">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
@@ -1118,7 +1115,7 @@
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="12.75" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>43</v>
       </c>
@@ -1152,7 +1149,7 @@
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="12.75" customHeight="1">
       <c r="A6" s="10" t="s">
         <v>43</v>
       </c>
@@ -1186,7 +1183,7 @@
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="12.75" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>34</v>
       </c>
@@ -1218,7 +1215,7 @@
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="12.75" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>35</v>
       </c>
@@ -1252,7 +1249,7 @@
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="12.75" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
@@ -1286,7 +1283,7 @@
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="12.75" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>36</v>
       </c>
@@ -1320,7 +1317,7 @@
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="14.25">
       <c r="A11" s="10" t="s">
         <v>39</v>
       </c>
@@ -1352,7 +1349,7 @@
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="14.25">
       <c r="A12" s="11" t="s">
         <v>37</v>
       </c>
@@ -1386,7 +1383,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="14.25">
       <c r="A13" s="11" t="s">
         <v>40</v>
       </c>
@@ -1420,7 +1417,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="14.25">
       <c r="A14" s="11" t="s">
         <v>41</v>
       </c>
@@ -1452,7 +1449,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="14.25">
       <c r="A15" s="11" t="s">
         <v>42</v>
       </c>
@@ -1484,7 +1481,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="14.25">
       <c r="A16" s="11" t="s">
         <v>43</v>
       </c>
@@ -1518,7 +1515,7 @@
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
     </row>
-    <row r="17" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="14.25">
       <c r="A17" s="11" t="s">
         <v>43</v>
       </c>
@@ -1552,7 +1549,7 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
     </row>
-    <row r="18" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="14.25">
       <c r="A18" s="11" t="s">
         <v>34</v>
       </c>
@@ -1584,7 +1581,7 @@
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
     </row>
-    <row r="19" spans="1:20" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="14.25">
       <c r="A19" s="10" t="s">
         <v>36</v>
       </c>
@@ -1618,7 +1615,7 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
     </row>
-    <row r="20" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="12.75" customHeight="1">
       <c r="A20" s="10" t="s">
         <v>39</v>
       </c>
@@ -1639,7 +1636,7 @@
       </c>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="12.75" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>41</v>
       </c>
@@ -1660,7 +1657,7 @@
       </c>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="12.75" customHeight="1">
       <c r="A22" s="11" t="s">
         <v>42</v>
       </c>
@@ -1681,7 +1678,7 @@
       </c>
       <c r="G22" s="4"/>
     </row>
-    <row r="23" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="12.75" customHeight="1">
       <c r="A23" s="10" t="s">
         <v>44</v>
       </c>
@@ -1702,7 +1699,7 @@
       </c>
       <c r="G23" s="4"/>
     </row>
-    <row r="24" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="12.75" customHeight="1">
       <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
@@ -1723,7 +1720,7 @@
       </c>
       <c r="G24" s="4"/>
     </row>
-    <row r="25" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="12.75" customHeight="1">
       <c r="A25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1744,7 +1741,7 @@
       </c>
       <c r="G25" s="4"/>
     </row>
-    <row r="26" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="12.75" customHeight="1">
       <c r="A26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1763,7 +1760,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row r="27" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="12.75" customHeight="1">
       <c r="A27" s="10" t="s">
         <v>47</v>
       </c>
@@ -1789,7 +1786,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="12.75" customHeight="1">
       <c r="A28" s="10" t="s">
         <v>49</v>
       </c>
@@ -1815,7 +1812,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="12.75" customHeight="1">
       <c r="A29" s="10" t="s">
         <v>50</v>
       </c>
@@ -1841,7 +1838,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="12.75" customHeight="1">
       <c r="A30" s="10"/>
       <c r="B30" s="18"/>
       <c r="C30" s="4" t="s">
@@ -1858,7 +1855,7 @@
       </c>
       <c r="G30" s="4"/>
     </row>
-    <row r="31" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="12.75" customHeight="1">
       <c r="B31" s="18"/>
       <c r="C31" s="14" t="s">
         <v>66</v>
@@ -1868,7 +1865,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
-    <row r="32" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="12.75" customHeight="1">
       <c r="B32" s="18">
         <v>41184</v>
       </c>
@@ -1891,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" customHeight="1">
       <c r="A33" s="10"/>
       <c r="B33" s="18">
         <v>41184</v>
@@ -1915,7 +1912,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" customHeight="1">
       <c r="A34" s="10"/>
       <c r="B34" s="18">
         <v>41184</v>
@@ -1939,7 +1936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="12.75" customHeight="1">
       <c r="A35" s="12"/>
       <c r="B35" s="18">
         <v>41184</v>
@@ -1963,7 +1960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="12.75" customHeight="1">
       <c r="A36" s="12"/>
       <c r="B36" s="18">
         <v>41184</v>
@@ -1987,7 +1984,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" customHeight="1">
       <c r="B37" s="18">
         <v>41184</v>
       </c>
@@ -2005,7 +2002,7 @@
       </c>
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" customHeight="1">
       <c r="A38" s="12"/>
       <c r="B38" s="18">
         <v>41184</v>
@@ -2023,7 +2020,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" customHeight="1">
       <c r="A39" s="12"/>
       <c r="B39" s="18">
         <v>41184</v>
@@ -2041,7 +2038,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" customHeight="1">
       <c r="A40" s="12"/>
       <c r="B40" s="18">
         <v>41184</v>
@@ -2059,7 +2056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" customHeight="1">
       <c r="A41" s="12"/>
       <c r="B41" s="18">
         <v>41184</v>
@@ -2080,7 +2077,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" customHeight="1">
       <c r="A42" s="12"/>
       <c r="B42" s="18">
         <v>41184</v>
@@ -2104,7 +2101,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" customHeight="1">
       <c r="A43" s="12"/>
       <c r="B43" s="18"/>
       <c r="C43" s="26" t="s">
@@ -2112,7 +2109,7 @@
       </c>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" customHeight="1">
       <c r="A44" s="12"/>
       <c r="B44" s="18"/>
       <c r="C44" s="16" t="s">
@@ -2134,7 +2131,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" customHeight="1">
       <c r="A45" s="12"/>
       <c r="B45" s="18"/>
       <c r="C45" s="16" t="s">
@@ -2156,20 +2153,23 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="12.75" customHeight="1">
       <c r="A46" s="12"/>
       <c r="B46" s="18"/>
       <c r="C46" s="16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E46" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="12.75" customHeight="1">
       <c r="A47" s="12"/>
       <c r="B47" s="18"/>
       <c r="C47" s="21" t="s">
@@ -2178,11 +2178,14 @@
       <c r="D47" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="E47" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E47" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="12.75" customHeight="1">
       <c r="A48" s="12"/>
       <c r="B48" s="18"/>
       <c r="C48" s="22" t="s">
@@ -2191,11 +2194,14 @@
       <c r="D48" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E48" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="12.75" customHeight="1">
       <c r="A49" s="12"/>
       <c r="B49" s="18"/>
       <c r="C49" s="22" t="s">
@@ -2204,11 +2210,14 @@
       <c r="D49" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E49" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="12.75" customHeight="1">
       <c r="A50" s="12"/>
       <c r="B50" s="18"/>
       <c r="C50" s="4" t="s">
@@ -2217,26 +2226,30 @@
       <c r="D50" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E50" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="20"/>
+      <c r="E50" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="12.75" customHeight="1">
       <c r="C51" s="22" t="s">
         <v>88</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="20"/>
+      <c r="E51" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="12.75" customHeight="1">
       <c r="C52" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>92</v>
@@ -2245,29 +2258,32 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="20"/>
+    <row r="53" spans="1:8" ht="12.75" customHeight="1">
       <c r="C53" s="25" t="s">
         <v>96</v>
       </c>
       <c r="E53" s="27"/>
     </row>
-    <row r="54" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="12.75" customHeight="1">
       <c r="A54" s="12"/>
-      <c r="B54" s="20"/>
       <c r="C54" s="21" t="s">
         <v>98</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E54" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="12.75" customHeight="1">
       <c r="A55" s="12"/>
-      <c r="B55" s="20"/>
       <c r="C55" s="21" t="s">
         <v>74</v>
       </c>
@@ -2278,33 +2294,40 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="12.75" customHeight="1">
       <c r="A56" s="12"/>
-      <c r="B56" s="20"/>
       <c r="C56" s="21" t="s">
         <v>97</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E56" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F56" t="s">
+        <v>92</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="12.75" customHeight="1">
       <c r="A57" s="12"/>
-      <c r="B57" s="20"/>
       <c r="C57" s="4" t="s">
         <v>83</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E57" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="12.75" customHeight="1">
       <c r="A58" s="12"/>
       <c r="B58" s="18"/>
       <c r="C58" s="22" t="s">
@@ -2317,89 +2340,53 @@
         <v>23</v>
       </c>
     </row>
-    <row r="59" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="12.75" customHeight="1">
       <c r="A59" s="12"/>
-      <c r="B59" s="20"/>
       <c r="C59" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="12.75" customHeight="1">
+      <c r="A60" s="12"/>
+      <c r="C60" s="21" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="12"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E60" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="12.75" customHeight="1">
       <c r="A61" s="12"/>
-      <c r="B61" s="20"/>
-    </row>
-    <row r="62" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:8" ht="12.75" customHeight="1">
       <c r="A62" s="12"/>
-      <c r="B62" s="20"/>
-    </row>
-    <row r="63" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:8" ht="12.75" customHeight="1">
       <c r="A63" s="12"/>
-      <c r="B63" s="20"/>
-    </row>
-    <row r="64" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:8" ht="12.75" customHeight="1">
       <c r="A64" s="12"/>
-      <c r="B64" s="20"/>
-    </row>
-    <row r="65" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:1" ht="12.75" customHeight="1">
       <c r="A65" s="12"/>
-      <c r="B65" s="20"/>
-    </row>
-    <row r="66" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:1" ht="12.75" customHeight="1">
       <c r="A66" s="12"/>
-      <c r="B66" s="20"/>
-    </row>
-    <row r="67" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:1" ht="12.75" customHeight="1">
       <c r="A67" s="12"/>
-      <c r="B67" s="20"/>
-    </row>
-    <row r="68" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:1" ht="12.75" customHeight="1">
       <c r="A68" s="12"/>
-      <c r="B68" s="20"/>
-    </row>
-    <row r="69" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:1" ht="12.75" customHeight="1">
       <c r="A69" s="12"/>
-      <c r="B69" s="20"/>
-    </row>
-    <row r="70" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:1" ht="12.75" customHeight="1">
       <c r="A70" s="12"/>
-      <c r="B70" s="20"/>
-    </row>
-    <row r="71" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="20"/>
-    </row>
-    <row r="72" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="20"/>
-    </row>
-    <row r="73" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="20"/>
-    </row>
-    <row r="74" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="20"/>
-    </row>
-    <row r="75" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="20"/>
-    </row>
-    <row r="76" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="20"/>
-    </row>
-    <row r="77" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="20"/>
-    </row>
-    <row r="78" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="20"/>
-    </row>
-    <row r="79" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="20"/>
-    </row>
-    <row r="80" spans="1:20" s="3" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>